<commit_message>
added some plots, enhanced eda plotting, as well as modeling code, and wrote some more modeling files for use in the final presentation.
</commit_message>
<xml_diff>
--- a/reports/lagged_weather_effects_results.xlsx
+++ b/reports/lagged_weather_effects_results.xlsx
@@ -19,14 +19,19 @@
     <sheet name="demand_resid ~ precip_lag1" sheetId="10" r:id="rId10"/>
     <sheet name="demand_resid ~ precip_lag2" sheetId="11" r:id="rId11"/>
     <sheet name="demand_resid ~ precip_lag3" sheetId="12" r:id="rId12"/>
-    <sheet name="demand_resid ~ wind_chill_f+pre" sheetId="13" r:id="rId13"/>
+    <sheet name="demand_resid ~ wind_chill_diff+" sheetId="13" r:id="rId13"/>
+    <sheet name="demand_resid ~ wind_chill_f+rai" sheetId="14" r:id="rId14"/>
+    <sheet name="demand_resid ~ wind_chill_f+win" sheetId="15" r:id="rId15"/>
+    <sheet name="demand_resid ~ rain_flag_lag1+p" sheetId="16" r:id="rId16"/>
+    <sheet name="demand_resid ~ wind_chill_f+pre" sheetId="17" r:id="rId17"/>
+    <sheet name="demand_resid ~ wind_chill_f+hea" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="85">
   <si>
     <t>model_label</t>
   </si>
@@ -91,6 +96,18 @@
     <t>p_4</t>
   </si>
   <si>
+    <t>coef_5</t>
+  </si>
+  <si>
+    <t>var_5</t>
+  </si>
+  <si>
+    <t>sig_5</t>
+  </si>
+  <si>
+    <t>p_5</t>
+  </si>
+  <si>
     <t>demand_resid ~ rain_flag_lag0</t>
   </si>
   <si>
@@ -154,13 +171,46 @@
     <t>demand_resid ~ precip_lag3</t>
   </si>
   <si>
+    <t>demand_resid ~ wind_chill_diff+rain_flag_lag0+rain_flag_lag1</t>
+  </si>
+  <si>
+    <t>demand_resid ~ rain_flag_lag0+rain_flag_lag1+heavy_rain_flag_lag0+heavy_rain_flag_lag1</t>
+  </si>
+  <si>
+    <t>demand_resid ~ wind_chill_f+rain_flag_lag0+rain_flag_lag1</t>
+  </si>
+  <si>
+    <t>demand_resid ~ wind_chill_f+wind_chill_diff</t>
+  </si>
+  <si>
+    <t>demand_resid ~ wind_chill_f+wind_chill_diff+precip_lag0+precip_lag1+precip_lag2</t>
+  </si>
+  <si>
+    <t>demand_resid ~ rain_flag_lag1+precip_lag0</t>
+  </si>
+  <si>
+    <t>demand_resid ~ heavy_rain_flag_lag0+precip_lag0</t>
+  </si>
+  <si>
+    <t>demand_resid ~ wind_chill_f+rain_flag_lag1+precip_lag0</t>
+  </si>
+  <si>
+    <t>demand_resid ~ wind_chill_diff+rain_flag_lag1+precip_lag0</t>
+  </si>
+  <si>
     <t>demand_resid ~ wind_chill_f+precip_lag0+rain_flag_lag0</t>
   </si>
   <si>
-    <t>demand_resid ~ wind_chill_f+precip_lag0+rain_flag_lag1</t>
-  </si>
-  <si>
-    <t>demand_resid ~ wind_chill_f+precip_lag1+rain_flag_lag0</t>
+    <t>demand_resid ~ wind_chill_f+heavy_rain_flag_lag0+precip_lag0</t>
+  </si>
+  <si>
+    <t>demand_resid ~ wind_chill_diff+heavy_rain_flag_lag1+precip_lag0</t>
+  </si>
+  <si>
+    <t>demand_resid ~ wind_chill_diff+heavy_rain_flag_lag0+heavy_rain_flag_lag1</t>
+  </si>
+  <si>
+    <t>demand_resid ~ wind_chill_diff+precip_lag0</t>
   </si>
   <si>
     <t>demand_resid</t>
@@ -202,6 +252,9 @@
     <t>precip_lag3</t>
   </si>
   <si>
+    <t>wind_chill_diff</t>
+  </si>
+  <si>
     <t>wind_chill_f</t>
   </si>
   <si>
@@ -212,6 +265,9 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
   <si>
     <t>param</t>
@@ -587,13 +643,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,13 +713,25 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C2">
         <v>0.008928657066125778</v>
@@ -678,21 +746,21 @@
         <v>-54.4834129276495</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I2">
         <v>8.700229480534171E-13</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>0.01182398598311907</v>
@@ -707,10 +775,10 @@
         <v>-27.24426302132451</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="I3">
         <v>0.007059423298074113</v>
@@ -719,21 +787,21 @@
         <v>-41.2781525442352</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="M3">
         <v>4.502087729084618E-05</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C4">
         <v>0.01184706733823104</v>
@@ -748,10 +816,10 @@
         <v>-26.66276727713015</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="I4">
         <v>0.009270716185017397</v>
@@ -760,10 +828,10 @@
         <v>-39.26750294337013</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="L4" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="M4">
         <v>0.0007125856861977624</v>
@@ -772,18 +840,18 @@
         <v>-3.632432719038859</v>
       </c>
       <c r="O4" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="Q4">
         <v>0.7229064312218962</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>0.01185989089616424</v>
@@ -798,10 +866,10 @@
         <v>-26.82300394988875</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="I5">
         <v>0.008958568333586308</v>
@@ -810,10 +878,10 @@
         <v>-39.68709488164458</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="M5">
         <v>0.0006807359339784485</v>
@@ -822,7 +890,7 @@
         <v>-5.375019499828974</v>
       </c>
       <c r="O5" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="Q5">
         <v>0.6452782099899299</v>
@@ -831,18 +899,18 @@
         <v>3.202375218635177</v>
       </c>
       <c r="S5" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="U5">
         <v>0.7549406277298476</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C6">
         <v>0.004523049610699825</v>
@@ -857,21 +925,21 @@
         <v>-139.1960535384449</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I6">
         <v>3.713831197155289E-07</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C7">
         <v>0.006710458301420696</v>
@@ -886,10 +954,10 @@
         <v>-106.735453874469</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I7">
         <v>0.0002150047080020909</v>
@@ -898,21 +966,21 @@
         <v>-102.0836227646419</v>
       </c>
       <c r="K7" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="L7" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="M7">
         <v>0.0004007411070565182</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C8">
         <v>0.00684662534492031</v>
@@ -927,10 +995,10 @@
         <v>-105.7646835040477</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I8">
         <v>0.0002482875701797903</v>
@@ -939,10 +1007,10 @@
         <v>-110.4961493368396</v>
       </c>
       <c r="K8" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="L8" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="M8">
         <v>0.0002755190264050106</v>
@@ -951,18 +1019,18 @@
         <v>25.46894884425286</v>
       </c>
       <c r="O8" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="Q8">
         <v>0.377336709088176</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C9">
         <v>0.006858701635833686</v>
@@ -977,10 +1045,10 @@
         <v>-105.627263911452</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I9">
         <v>0.0002539977918181738</v>
@@ -989,10 +1057,10 @@
         <v>-110.2353487124659</v>
       </c>
       <c r="K9" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="L9" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="M9">
         <v>0.0002873970206090095</v>
@@ -1001,7 +1069,7 @@
         <v>22.90131473069702</v>
       </c>
       <c r="O9" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="Q9">
         <v>0.4509699234018555</v>
@@ -1010,18 +1078,18 @@
         <v>7.814599595548566</v>
       </c>
       <c r="S9" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="U9">
         <v>0.7865435476558567</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C10">
         <v>0.006158244860145157</v>
@@ -1036,21 +1104,21 @@
         <v>-10.61904168729323</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I10">
         <v>2.963893809329023E-09</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C11">
         <v>0.01178289045379399</v>
@@ -1065,10 +1133,10 @@
         <v>-7.722589253615498</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I11">
         <v>3.1317985541802E-05</v>
@@ -1077,21 +1145,21 @@
         <v>-10.55275661263593</v>
       </c>
       <c r="K11" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="L11" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="M11">
         <v>1.301891690767532E-08</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C12">
         <v>0.01282781699395952</v>
@@ -1106,10 +1174,10 @@
         <v>-7.490519945034891</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I12">
         <v>5.462617443758573E-05</v>
@@ -1118,10 +1186,10 @@
         <v>-9.366454819246124</v>
       </c>
       <c r="K12" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="M12">
         <v>1.025363531644206E-06</v>
@@ -1130,21 +1198,21 @@
         <v>-4.553670685183396</v>
       </c>
       <c r="O12" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="P12" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="Q12">
         <v>0.01412698769448066</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C13">
         <v>0.01285355731058779</v>
@@ -1159,10 +1227,10 @@
         <v>-7.510461496580619</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I13">
         <v>5.266911023400927E-05</v>
@@ -1171,10 +1239,10 @@
         <v>-9.398405708192845</v>
       </c>
       <c r="K13" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="L13" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="M13">
         <v>9.670927558909536E-07</v>
@@ -1183,10 +1251,10 @@
         <v>-4.745769310353319</v>
       </c>
       <c r="O13" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="P13" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="Q13">
         <v>0.01331166225493849</v>
@@ -1195,18 +1263,18 @@
         <v>0.7442957421406289</v>
       </c>
       <c r="S13" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="U13">
         <v>0.6884228342218432</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C14">
         <v>0.008928657066125778</v>
@@ -1221,21 +1289,21 @@
         <v>-54.4834129276495</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H14" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I14">
         <v>8.700229480534171E-13</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C15">
         <v>0.01056439128535491</v>
@@ -1250,21 +1318,21 @@
         <v>-59.26392402074157</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I15">
         <v>7.278140773706735E-15</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C16">
         <v>0.005715785366040116</v>
@@ -1279,21 +1347,21 @@
         <v>-43.59217452162888</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H16" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I16">
         <v>1.098232356866827E-08</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C17">
         <v>0.003210521371698416</v>
@@ -1308,21 +1376,21 @@
         <v>-32.6704322645726</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="H17" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I17">
         <v>1.869171859097764E-05</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C18">
         <v>0.004523049610699825</v>
@@ -1337,21 +1405,21 @@
         <v>-139.1960535384449</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="H18" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I18">
         <v>3.713831197155289E-07</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C19">
         <v>0.00431999777318115</v>
@@ -1366,21 +1434,21 @@
         <v>-136.033969060426</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H19" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I19">
         <v>6.800552881945479E-07</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C20">
         <v>6.547575630910796E-05</v>
@@ -1395,18 +1463,18 @@
         <v>-16.74733515722549</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="I20">
         <v>0.5413408300192777</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C21">
         <v>1.589707984250843E-05</v>
@@ -1421,18 +1489,18 @@
         <v>8.251978281442831</v>
       </c>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="I21">
         <v>0.7634684174019746</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C22">
         <v>0.006158244860145157</v>
@@ -1447,21 +1515,21 @@
         <v>-10.61904168729323</v>
       </c>
       <c r="G22" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I22">
         <v>2.963893809329023E-09</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C23">
         <v>0.008771407388207364</v>
@@ -1476,21 +1544,21 @@
         <v>-12.67319624774046</v>
       </c>
       <c r="G23" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="H23" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I23">
         <v>1.385387241453708E-12</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C24">
         <v>0.003533350427943782</v>
@@ -1505,21 +1573,21 @@
         <v>-8.043499237610394</v>
       </c>
       <c r="G24" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I24">
         <v>7.096990357906783E-06</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C25">
         <v>0.0002761185798996202</v>
@@ -1534,163 +1602,710 @@
         <v>-2.248504400515804</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I25">
         <v>0.2097535223016775</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C26">
-        <v>0.03516259729642923</v>
+        <v>0.03431369901755899</v>
       </c>
       <c r="D26">
-        <v>0.03353920290040524</v>
+        <v>0.03268796450412048</v>
       </c>
       <c r="E26">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="F26">
-        <v>-0.7430586436820985</v>
+        <v>-1.687619621028324</v>
       </c>
       <c r="G26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26">
+        <v>0.1068178493641185</v>
+      </c>
+      <c r="J26">
+        <v>-45.39083353615307</v>
+      </c>
+      <c r="K26" t="s">
+        <v>61</v>
+      </c>
+      <c r="L26" t="s">
+        <v>76</v>
+      </c>
+      <c r="M26">
+        <v>0.005416927846441815</v>
+      </c>
+      <c r="N26">
+        <v>-41.39253603073699</v>
+      </c>
+      <c r="O26" t="s">
+        <v>64</v>
+      </c>
+      <c r="P26" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q26">
+        <v>0.01102458511551744</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
         <v>60</v>
       </c>
-      <c r="I26">
-        <v>0.005007503611045534</v>
-      </c>
-      <c r="J26">
-        <v>-8.180970027785605</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="C27">
+        <v>0.01446016154175256</v>
+      </c>
+      <c r="D27">
+        <v>0.01376806895856564</v>
+      </c>
+      <c r="E27">
+        <v>5701</v>
+      </c>
+      <c r="F27">
+        <v>-21.74897429114493</v>
+      </c>
+      <c r="G27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27">
+        <v>0.03432590023048793</v>
+      </c>
+      <c r="J27">
+        <v>-36.35860384236335</v>
+      </c>
+      <c r="K27" t="s">
+        <v>64</v>
+      </c>
+      <c r="L27" t="s">
+        <v>75</v>
+      </c>
+      <c r="M27">
+        <v>0.0004054293854308489</v>
+      </c>
+      <c r="N27">
+        <v>-73.65374922066619</v>
+      </c>
+      <c r="O27" t="s">
+        <v>62</v>
+      </c>
+      <c r="P27" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q27">
+        <v>0.01231211502222284</v>
+      </c>
+      <c r="R27">
+        <v>-63.61942301302211</v>
+      </c>
+      <c r="S27" t="s">
+        <v>67</v>
+      </c>
+      <c r="T27" t="s">
+        <v>77</v>
+      </c>
+      <c r="U27">
+        <v>0.0306018668488323</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25">
+      <c r="A28" t="s">
         <v>48</v>
       </c>
-      <c r="M26">
-        <v>0.1033917261919767</v>
-      </c>
-      <c r="N26">
-        <v>-64.12778379854394</v>
-      </c>
-      <c r="O26" t="s">
-        <v>46</v>
-      </c>
-      <c r="P26" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q26">
-        <v>4.78298189506248E-07</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="A27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27">
-        <v>0.03547649237896067</v>
-      </c>
-      <c r="D27">
-        <v>0.0338527154301036</v>
-      </c>
-      <c r="E27">
-        <v>1786</v>
-      </c>
-      <c r="F27">
-        <v>-0.7132605283945157</v>
-      </c>
-      <c r="G27" t="s">
-        <v>58</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="B28" t="s">
         <v>60</v>
       </c>
-      <c r="I27">
-        <v>0.007145974443627691</v>
-      </c>
-      <c r="J27">
-        <v>-10.37437994905635</v>
-      </c>
-      <c r="K27" t="s">
-        <v>48</v>
-      </c>
-      <c r="L27" t="s">
-        <v>61</v>
-      </c>
-      <c r="M27">
-        <v>0.03042781593439595</v>
-      </c>
-      <c r="N27">
-        <v>-61.79723016719007</v>
-      </c>
-      <c r="O27" t="s">
-        <v>49</v>
-      </c>
-      <c r="P27" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q27">
-        <v>3.472548940533771E-07</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="A28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
       <c r="C28">
-        <v>0.03381630681318115</v>
+        <v>0.03703663456390049</v>
       </c>
       <c r="D28">
-        <v>0.03218973493912924</v>
+        <v>0.03541548411703832</v>
       </c>
       <c r="E28">
         <v>1786</v>
       </c>
       <c r="F28">
-        <v>-0.7566901384448409</v>
+        <v>-0.7308874287519651</v>
       </c>
       <c r="G28" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28">
+        <v>0.005737178083232345</v>
+      </c>
+      <c r="J28">
+        <v>-44.84214509464686</v>
+      </c>
+      <c r="K28" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28" t="s">
+        <v>76</v>
+      </c>
+      <c r="M28">
+        <v>0.005938354280064577</v>
+      </c>
+      <c r="N28">
+        <v>-40.29821967996101</v>
+      </c>
+      <c r="O28" t="s">
+        <v>64</v>
+      </c>
+      <c r="P28" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q28">
+        <v>0.01322045201113992</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29">
+        <v>0.007670399316416998</v>
+      </c>
+      <c r="D29">
+        <v>0.006557922185605802</v>
+      </c>
+      <c r="E29">
+        <v>1787</v>
+      </c>
+      <c r="F29">
+        <v>-1.410325843542292</v>
+      </c>
+      <c r="G29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s">
+        <v>76</v>
+      </c>
+      <c r="I29">
+        <v>0.003497253962379982</v>
+      </c>
+      <c r="J29">
+        <v>2.237454394839795</v>
+      </c>
+      <c r="K29" t="s">
+        <v>73</v>
+      </c>
+      <c r="M29">
+        <v>0.2411640753224102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30">
+        <v>0.02281678252210273</v>
+      </c>
+      <c r="D30">
+        <v>0.02007034290018628</v>
+      </c>
+      <c r="E30">
+        <v>1785</v>
+      </c>
+      <c r="F30">
+        <v>-1.288309174520416</v>
+      </c>
+      <c r="G30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30">
+        <v>0.007333756696862163</v>
+      </c>
+      <c r="J30">
+        <v>2.407570268082588</v>
+      </c>
+      <c r="K30" t="s">
+        <v>73</v>
+      </c>
+      <c r="M30">
+        <v>0.2047868450431195</v>
+      </c>
+      <c r="N30">
+        <v>-20.79600612927525</v>
+      </c>
+      <c r="O30" t="s">
+        <v>63</v>
+      </c>
+      <c r="P30" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q30">
+        <v>0.0001740235484464135</v>
+      </c>
+      <c r="R30">
+        <v>1.850335831084409</v>
+      </c>
+      <c r="S30" t="s">
+        <v>70</v>
+      </c>
+      <c r="U30">
+        <v>0.8021327263945893</v>
+      </c>
+      <c r="V30">
+        <v>-6.965119262557973</v>
+      </c>
+      <c r="W30" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y30">
+        <v>0.3434977546103082</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31">
+        <v>0.01309767491877134</v>
+      </c>
+      <c r="D31">
+        <v>0.01275127185626479</v>
+      </c>
+      <c r="E31">
+        <v>5701</v>
+      </c>
+      <c r="F31">
+        <v>-50.27710636068223</v>
+      </c>
+      <c r="G31" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I31">
+        <v>2.654133156104596E-10</v>
+      </c>
+      <c r="J31">
+        <v>-7.129806023013639</v>
+      </c>
+      <c r="K31" t="s">
+        <v>63</v>
+      </c>
+      <c r="L31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M31">
+        <v>0.0001324781015955244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <v>0.006425233444833145</v>
+      </c>
+      <c r="D32">
+        <v>0.006076549547112453</v>
+      </c>
+      <c r="E32">
+        <v>5702</v>
+      </c>
+      <c r="F32">
+        <v>-48.05782522497432</v>
+      </c>
+      <c r="G32" t="s">
+        <v>62</v>
+      </c>
+      <c r="I32">
+        <v>0.2159522958925692</v>
+      </c>
+      <c r="J32">
+        <v>-8.386671121593157</v>
+      </c>
+      <c r="K32" t="s">
+        <v>63</v>
+      </c>
+      <c r="L32" t="s">
+        <v>75</v>
+      </c>
+      <c r="M32">
+        <v>0.0009620257160912005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33">
+        <v>0.03547649237896067</v>
+      </c>
+      <c r="D33">
+        <v>0.0338527154301036</v>
+      </c>
+      <c r="E33">
+        <v>1786</v>
+      </c>
+      <c r="F33">
+        <v>-0.7132605283945155</v>
+      </c>
+      <c r="G33" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33">
+        <v>0.007145974443627684</v>
+      </c>
+      <c r="J33">
+        <v>-61.79723016719001</v>
+      </c>
+      <c r="K33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L33" t="s">
+        <v>75</v>
+      </c>
+      <c r="M33">
+        <v>3.472548940533784E-07</v>
+      </c>
+      <c r="N33">
+        <v>-10.37437994905637</v>
+      </c>
+      <c r="O33" t="s">
+        <v>63</v>
+      </c>
+      <c r="P33" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q33">
+        <v>0.03042781593439569</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34">
+        <v>0.03282429384425656</v>
+      </c>
+      <c r="D34">
+        <v>0.03119605191470143</v>
+      </c>
+      <c r="E34">
+        <v>1786</v>
+      </c>
+      <c r="F34">
+        <v>-1.605453754672248</v>
+      </c>
+      <c r="G34" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34">
+        <v>0.1257704276917745</v>
+      </c>
+      <c r="J34">
+        <v>-62.89528473448645</v>
+      </c>
+      <c r="K34" t="s">
+        <v>64</v>
+      </c>
+      <c r="L34" t="s">
+        <v>75</v>
+      </c>
+      <c r="M34">
+        <v>2.197631691680923E-07</v>
+      </c>
+      <c r="N34">
+        <v>-10.71887416698295</v>
+      </c>
+      <c r="O34" t="s">
+        <v>63</v>
+      </c>
+      <c r="P34" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q34">
+        <v>0.02550646964154965</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35">
+        <v>0.03516259729642923</v>
+      </c>
+      <c r="D35">
+        <v>0.03353920290040524</v>
+      </c>
+      <c r="E35">
+        <v>1787</v>
+      </c>
+      <c r="F35">
+        <v>-0.7430586436820985</v>
+      </c>
+      <c r="G35" t="s">
+        <v>74</v>
+      </c>
+      <c r="H35" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35">
+        <v>0.005007503611045534</v>
+      </c>
+      <c r="J35">
+        <v>-8.180970027785605</v>
+      </c>
+      <c r="K35" t="s">
+        <v>63</v>
+      </c>
+      <c r="M35">
+        <v>0.1033917261919767</v>
+      </c>
+      <c r="N35">
+        <v>-64.12778379854394</v>
+      </c>
+      <c r="O35" t="s">
+        <v>61</v>
+      </c>
+      <c r="P35" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q35">
+        <v>4.78298189506248E-07</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36">
+        <v>0.03734420550886441</v>
+      </c>
+      <c r="D36">
+        <v>0.03572448179407273</v>
+      </c>
+      <c r="E36">
+        <v>1787</v>
+      </c>
+      <c r="F36">
+        <v>-0.8095753284909452</v>
+      </c>
+      <c r="G36" t="s">
+        <v>74</v>
+      </c>
+      <c r="H36" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36">
+        <v>0.002185848504304497</v>
+      </c>
+      <c r="J36">
+        <v>431.2119723974194</v>
+      </c>
+      <c r="K36" t="s">
+        <v>62</v>
+      </c>
+      <c r="L36" t="s">
+        <v>75</v>
+      </c>
+      <c r="M36">
+        <v>5.935302640075449E-08</v>
+      </c>
+      <c r="N36">
+        <v>-53.41862211706037</v>
+      </c>
+      <c r="O36" t="s">
+        <v>63</v>
+      </c>
+      <c r="P36" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q36">
+        <v>1.50047644879816E-13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>0.02268382832669658</v>
+      </c>
+      <c r="D37">
+        <v>0.0210385149063711</v>
+      </c>
+      <c r="E37">
+        <v>1786</v>
+      </c>
+      <c r="F37">
+        <v>-2.068038037239637</v>
+      </c>
+      <c r="G37" t="s">
+        <v>73</v>
+      </c>
+      <c r="H37" t="s">
+        <v>77</v>
+      </c>
+      <c r="I37">
+        <v>0.04983155963767551</v>
+      </c>
+      <c r="J37">
+        <v>160.0287755350158</v>
+      </c>
+      <c r="K37" t="s">
+        <v>67</v>
+      </c>
+      <c r="L37" t="s">
+        <v>76</v>
+      </c>
+      <c r="M37">
+        <v>0.004030852586802127</v>
+      </c>
+      <c r="N37">
+        <v>-30.13973358405143</v>
+      </c>
+      <c r="O37" t="s">
+        <v>63</v>
+      </c>
+      <c r="P37" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q37">
+        <v>2.405619850996245E-09</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" t="s">
         <v>58</v>
       </c>
-      <c r="H28" t="s">
+      <c r="B38" t="s">
         <v>60</v>
       </c>
-      <c r="I28">
-        <v>0.004355226900948312</v>
-      </c>
-      <c r="J28">
-        <v>-2.088157067969264</v>
-      </c>
-      <c r="K28" t="s">
-        <v>55</v>
-      </c>
-      <c r="M28">
-        <v>0.6615538298618615</v>
-      </c>
-      <c r="N28">
-        <v>-72.86527464421842</v>
-      </c>
-      <c r="O28" t="s">
-        <v>46</v>
-      </c>
-      <c r="P28" t="s">
+      <c r="C38">
+        <v>0.003562800521340725</v>
+      </c>
+      <c r="D38">
+        <v>0.001885296818514681</v>
+      </c>
+      <c r="E38">
+        <v>1786</v>
+      </c>
+      <c r="F38">
+        <v>-2.328740649420762</v>
+      </c>
+      <c r="G38" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38">
+        <v>0.02863713496849756</v>
+      </c>
+      <c r="J38">
+        <v>-60.29772748043852</v>
+      </c>
+      <c r="K38" t="s">
+        <v>62</v>
+      </c>
+      <c r="M38">
+        <v>0.2952038544644854</v>
+      </c>
+      <c r="N38">
+        <v>16.8707750243922</v>
+      </c>
+      <c r="O38" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q38">
+        <v>0.7698859443514176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" t="s">
         <v>59</v>
       </c>
-      <c r="Q28">
-        <v>1.903060331504702E-09</v>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39">
+        <v>0.0181582243870988</v>
+      </c>
+      <c r="D39">
+        <v>0.01705750490771207</v>
+      </c>
+      <c r="E39">
+        <v>1787</v>
+      </c>
+      <c r="F39">
+        <v>-1.918053179839857</v>
+      </c>
+      <c r="G39" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39">
+        <v>0.06872154612822605</v>
+      </c>
+      <c r="J39">
+        <v>-22.43002134178147</v>
+      </c>
+      <c r="K39" t="s">
+        <v>63</v>
+      </c>
+      <c r="L39" t="s">
+        <v>75</v>
+      </c>
+      <c r="M39">
+        <v>1.58896732276653E-07</v>
       </c>
     </row>
   </sheetData>
@@ -1708,24 +2323,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>1.556895856856413</v>
@@ -1742,7 +2357,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>-12.67319624774046</v>
@@ -1772,24 +2387,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>0.994358203238384</v>
@@ -1806,7 +2421,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B3">
         <v>-8.043499237610394</v>
@@ -1836,24 +2451,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>0.2766338898084024</v>
@@ -1870,7 +2485,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B3">
         <v>-2.248504400515804</v>
@@ -1900,87 +2515,594 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
-        <v>26.51123233144472</v>
+        <v>-11.42125585752292</v>
       </c>
       <c r="C2">
-        <v>8.602725472989627</v>
+        <v>6.78010186534195</v>
       </c>
       <c r="D2">
-        <v>3.0817247876482</v>
+        <v>-1.684525702468467</v>
       </c>
       <c r="E2">
-        <v>0.002089556811299653</v>
+        <v>0.09225503246322896</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B3">
-        <v>-0.7566901384448409</v>
+        <v>-1.918053179839857</v>
       </c>
       <c r="C3">
-        <v>0.2650521290775134</v>
+        <v>1.053096010668639</v>
       </c>
       <c r="D3">
-        <v>-2.854872892658598</v>
+        <v>-1.821346924125212</v>
       </c>
       <c r="E3">
-        <v>0.004355226900948312</v>
+        <v>0.06872154612822605</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B4">
-        <v>-2.088157067969264</v>
+        <v>-22.43002134178147</v>
       </c>
       <c r="C4">
-        <v>4.769201445639064</v>
+        <v>4.261886857670911</v>
       </c>
       <c r="D4">
-        <v>-0.4378420772892002</v>
+        <v>-5.262932145045095</v>
       </c>
       <c r="E4">
-        <v>0.6615538298618615</v>
+        <v>1.58896732276653E-07</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B5">
-        <v>-72.86527464421842</v>
+        <v>16.8707750243922</v>
       </c>
       <c r="C5">
-        <v>12.06928844019226</v>
+        <v>57.66433065716832</v>
       </c>
       <c r="D5">
-        <v>-6.037246935085902</v>
+        <v>0.2925686439454921</v>
       </c>
       <c r="E5">
-        <v>1.903060331504702E-09</v>
+        <v>0.7698859443514176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2">
+        <v>25.23348980029696</v>
+      </c>
+      <c r="C2">
+        <v>8.58858284219219</v>
+      </c>
+      <c r="D2">
+        <v>2.938027176769508</v>
+      </c>
+      <c r="E2">
+        <v>0.003345519351431104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3">
+        <v>-0.7132605283945155</v>
+      </c>
+      <c r="C3">
+        <v>0.264849822796656</v>
+      </c>
+      <c r="D3">
+        <v>-2.693075346862272</v>
+      </c>
+      <c r="E3">
+        <v>0.007145974443627684</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4">
+        <v>-61.79723016719001</v>
+      </c>
+      <c r="C4">
+        <v>12.08121202302374</v>
+      </c>
+      <c r="D4">
+        <v>-5.115151530278593</v>
+      </c>
+      <c r="E4">
+        <v>3.472548940533784E-07</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5">
+        <v>-10.37437994905637</v>
+      </c>
+      <c r="C5">
+        <v>4.789198288290991</v>
+      </c>
+      <c r="D5">
+        <v>-2.16620388728119</v>
+      </c>
+      <c r="E5">
+        <v>0.03042781593439569</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2">
+        <v>53.34113560637128</v>
+      </c>
+      <c r="C2">
+        <v>24.72962420996072</v>
+      </c>
+      <c r="D2">
+        <v>2.156973157112767</v>
+      </c>
+      <c r="E2">
+        <v>0.0311413326668704</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3">
+        <v>-1.288309174520416</v>
+      </c>
+      <c r="C3">
+        <v>0.4799270759354207</v>
+      </c>
+      <c r="D3">
+        <v>-2.684385272511218</v>
+      </c>
+      <c r="E3">
+        <v>0.007333756696862163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4">
+        <v>2.407570268082588</v>
+      </c>
+      <c r="C4">
+        <v>1.89797231867241</v>
+      </c>
+      <c r="D4">
+        <v>1.268495986162027</v>
+      </c>
+      <c r="E4">
+        <v>0.2047868450431195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5">
+        <v>-20.79600612927525</v>
+      </c>
+      <c r="C5">
+        <v>5.527921924589209</v>
+      </c>
+      <c r="D5">
+        <v>-3.761993460285828</v>
+      </c>
+      <c r="E5">
+        <v>0.0001740235484464135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>1.850335831084409</v>
+      </c>
+      <c r="C6">
+        <v>7.382875977486548</v>
+      </c>
+      <c r="D6">
+        <v>0.2506253439346469</v>
+      </c>
+      <c r="E6">
+        <v>0.8021327263945893</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7">
+        <v>-6.965119262557973</v>
+      </c>
+      <c r="C7">
+        <v>7.350821044646514</v>
+      </c>
+      <c r="D7">
+        <v>-0.9475294283800527</v>
+      </c>
+      <c r="E7">
+        <v>0.3434977546103082</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2">
+        <v>4.275548846064483</v>
+      </c>
+      <c r="C2">
+        <v>1.973165974571209</v>
+      </c>
+      <c r="D2">
+        <v>2.166847037281598</v>
+      </c>
+      <c r="E2">
+        <v>0.03028782554371725</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>-50.27710636068223</v>
+      </c>
+      <c r="C3">
+        <v>7.943800250441118</v>
+      </c>
+      <c r="D3">
+        <v>-6.329100024624907</v>
+      </c>
+      <c r="E3">
+        <v>2.654133156104596E-10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4">
+        <v>-7.129806023013639</v>
+      </c>
+      <c r="C4">
+        <v>1.864282270213634</v>
+      </c>
+      <c r="D4">
+        <v>-3.824424089060618</v>
+      </c>
+      <c r="E4">
+        <v>0.0001324781015955244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2">
+        <v>26.03046333049348</v>
+      </c>
+      <c r="C2">
+        <v>8.591146402630814</v>
+      </c>
+      <c r="D2">
+        <v>3.029917325413326</v>
+      </c>
+      <c r="E2">
+        <v>0.002481371011611148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3">
+        <v>-0.7430586436820985</v>
+      </c>
+      <c r="C3">
+        <v>0.264429178989241</v>
+      </c>
+      <c r="D3">
+        <v>-2.810047841627689</v>
+      </c>
+      <c r="E3">
+        <v>0.005007503611045534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4">
+        <v>-8.180970027785605</v>
+      </c>
+      <c r="C4">
+        <v>5.020654685622923</v>
+      </c>
+      <c r="D4">
+        <v>-1.629462797195058</v>
+      </c>
+      <c r="E4">
+        <v>0.1033917261919767</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>-64.12778379854394</v>
+      </c>
+      <c r="C5">
+        <v>12.68982350315872</v>
+      </c>
+      <c r="D5">
+        <v>-5.053481144365912</v>
+      </c>
+      <c r="E5">
+        <v>4.78298189506248E-07</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2">
+        <v>26.22012732091926</v>
+      </c>
+      <c r="C2">
+        <v>8.581829976185739</v>
+      </c>
+      <c r="D2">
+        <v>3.055307247251361</v>
+      </c>
+      <c r="E2">
+        <v>0.002281626955929964</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3">
+        <v>-0.8095753284909452</v>
+      </c>
+      <c r="C3">
+        <v>0.2638588911719245</v>
+      </c>
+      <c r="D3">
+        <v>-3.068213183551371</v>
+      </c>
+      <c r="E3">
+        <v>0.002185848504304497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <v>431.2119723974194</v>
+      </c>
+      <c r="C4">
+        <v>79.20984837529733</v>
+      </c>
+      <c r="D4">
+        <v>5.443918669738279</v>
+      </c>
+      <c r="E4">
+        <v>5.935302640075449E-08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5">
+        <v>-53.41862211706037</v>
+      </c>
+      <c r="C5">
+        <v>7.175045680950983</v>
+      </c>
+      <c r="D5">
+        <v>-7.445056727496715</v>
+      </c>
+      <c r="E5">
+        <v>1.50047644879816E-13</v>
       </c>
     </row>
   </sheetData>
@@ -1998,24 +3120,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>3.678729213810149</v>
@@ -2032,7 +3154,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <v>-54.4834129276495</v>
@@ -2062,104 +3184,104 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
-        <v>4.641982527478343</v>
+        <v>4.608253361704927</v>
       </c>
       <c r="C2">
-        <v>2.006396241117056</v>
+        <v>1.984537919017312</v>
       </c>
       <c r="D2">
-        <v>2.313592117225026</v>
+        <v>2.32207876581507</v>
       </c>
       <c r="E2">
-        <v>0.02072554679247185</v>
+        <v>0.02026377615278022</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B3">
-        <v>-26.82300394988875</v>
+        <v>-21.74897429114493</v>
       </c>
       <c r="C3">
-        <v>10.25920631456961</v>
+        <v>10.27479209927992</v>
       </c>
       <c r="D3">
-        <v>-2.61453012323147</v>
+        <v>-2.11673132468239</v>
       </c>
       <c r="E3">
-        <v>0.008958568333586308</v>
+        <v>0.03432590023048793</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B4">
-        <v>-39.68709488164458</v>
+        <v>-36.35860384236335</v>
       </c>
       <c r="C4">
-        <v>11.67578609589558</v>
+        <v>10.27479209927993</v>
       </c>
       <c r="D4">
-        <v>-3.399094035783671</v>
+        <v>-3.538621851522564</v>
       </c>
       <c r="E4">
-        <v>0.0006807359339784485</v>
+        <v>0.0004054293854308489</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B5">
-        <v>-5.375019499828974</v>
+        <v>-73.65374922066619</v>
       </c>
       <c r="C5">
-        <v>11.67578609589558</v>
+        <v>29.41598099839493</v>
       </c>
       <c r="D5">
-        <v>-0.4603561127004948</v>
+        <v>-2.50386853406946</v>
       </c>
       <c r="E5">
-        <v>0.6452782099899299</v>
+        <v>0.01231211502222284</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B6">
-        <v>3.202375218635177</v>
+        <v>-63.61942301302211</v>
       </c>
       <c r="C6">
-        <v>10.25920631456963</v>
+        <v>29.41598099839496</v>
       </c>
       <c r="D6">
-        <v>0.3121464877928536</v>
+        <v>-2.162750343648013</v>
       </c>
       <c r="E6">
-        <v>0.7549406277298476</v>
+        <v>0.0306018668488323</v>
       </c>
     </row>
   </sheetData>
@@ -2177,75 +3299,75 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
-        <v>-0.03847219971596072</v>
+        <v>1.259541132903605</v>
       </c>
       <c r="C2">
-        <v>1.921996196791931</v>
+        <v>1.922962209924537</v>
       </c>
       <c r="D2">
-        <v>-0.02001679284286617</v>
+        <v>0.6550004604370431</v>
       </c>
       <c r="E2">
-        <v>0.9840306774781227</v>
+        <v>0.5124938931113161</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B3">
-        <v>8.251978281442831</v>
+        <v>-48.05782522497432</v>
       </c>
       <c r="C3">
-        <v>27.42034007771469</v>
+        <v>38.8345891830873</v>
       </c>
       <c r="D3">
-        <v>0.3009436884464264</v>
+        <v>-1.237500543610844</v>
       </c>
       <c r="E3">
-        <v>0.7634684174019746</v>
+        <v>0.2159522958925692</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B4">
-        <v>-110.2353487124659</v>
+        <v>-8.386671121593157</v>
       </c>
       <c r="C4">
-        <v>30.37910350013289</v>
+        <v>2.5390094524468</v>
       </c>
       <c r="D4">
-        <v>-3.62865707054139</v>
+        <v>-3.303127175643661</v>
       </c>
       <c r="E4">
-        <v>0.0002873970206090095</v>
+        <v>0.0009620257160912005</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <v>22.90131473069702</v>
@@ -2262,7 +3384,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B6">
         <v>7.814599595548566</v>
@@ -2292,24 +3414,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>1.29599984394735</v>
@@ -2326,7 +3448,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>-10.61904168729323</v>
@@ -2356,24 +3478,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>2.555414716550305</v>
@@ -2390,7 +3512,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>-7.510461496580619</v>
@@ -2407,7 +3529,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B4">
         <v>-9.398405708192845</v>
@@ -2424,7 +3546,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B5">
         <v>-4.745769310353319</v>
@@ -2441,7 +3563,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>0.7442957421406289</v>
@@ -2471,24 +3593,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>4.012137652889202</v>
@@ -2505,7 +3627,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>-59.26392402074157</v>
@@ -2535,24 +3657,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>2.956729443830317</v>
@@ -2569,7 +3691,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B3">
         <v>-43.59217452162888</v>
@@ -2599,24 +3721,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>2.20914524435157</v>
@@ -2633,7 +3755,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B3">
         <v>-32.6704322645726</v>

</xml_diff>